<commit_message>
workinng on template sheet
</commit_message>
<xml_diff>
--- a/public/hello world.xlsx
+++ b/public/hello world.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>CLIENT:</t>
   </si>
   <si>
-    <t>OPTP</t>
+    <t>MC  Donalds</t>
   </si>
   <si>
     <t>Prepared By:</t>
@@ -32,7 +32,7 @@
     <t>PERIOD:</t>
   </si>
   <si>
-    <t>2021-06-30</t>
+    <t>Jun 30 2022</t>
   </si>
   <si>
     <t>Reviewed By:</t>
@@ -92,59 +92,55 @@
     <t>SAVING</t>
   </si>
   <si>
+    <t>PKR</t>
+  </si>
+  <si>
+    <t>Clifton</t>
+  </si>
+  <si>
+    <t>May 17, 2021</t>
+  </si>
+  <si>
+    <t>MEEZAN BANK</t>
+  </si>
+  <si>
     <t>$</t>
   </si>
   <si>
-    <t>Clifton</t>
-  </si>
-  <si>
-    <t>May 17, 2021</t>
-  </si>
-  <si>
-    <t>January 6, 2021</t>
-  </si>
-  <si>
-    <t>December 14, 2021</t>
-  </si>
-  <si>
-    <t>June 20, 2021</t>
-  </si>
-  <si>
-    <t>MEEZAN BANK</t>
-  </si>
-  <si>
-    <t>ASAAN</t>
+    <t>Saddar</t>
+  </si>
+  <si>
+    <t>ALBARAKA</t>
+  </si>
+  <si>
+    <t>CURRENT</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>Saddar</t>
-  </si>
-  <si>
-    <t>ALBARAKA</t>
-  </si>
-  <si>
     <t>Kemari</t>
-  </si>
-  <si>
-    <t>SUMMIT BANK</t>
-  </si>
-  <si>
-    <t>DHA</t>
-  </si>
-  <si>
-    <t>May 18, 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -179,8 +175,13 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
     <border>
       <left style="thick">
         <color rgb="FF484848"/>
@@ -199,20 +200,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="4" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="2" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -514,10 +524,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,94 +550,99 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:15">
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="L3" s="2"/>
       <c r="N3" t="s">
         <v>3</v>
       </c>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="L4" s="2"/>
       <c r="N4" t="s">
         <v>3</v>
       </c>
+      <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="B9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9">
-        <v>10102</v>
+        <v>10201</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -639,60 +654,51 @@
         <v>26</v>
       </c>
       <c r="H9" s="1">
-        <v>1000.0</v>
+        <v>5000.0</v>
       </c>
       <c r="I9" s="1">
-        <v>6000.0</v>
+        <v>2000.0</v>
       </c>
       <c r="J9" s="1">
-        <v>6000.0</v>
+        <v>3000.0</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>-1000.0</v>
       </c>
       <c r="L9" t="s">
         <v>27</v>
-      </c>
-      <c r="M9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="B10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>10203</v>
+        <v>10205</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H10" s="1">
+        <v>-600.0</v>
+      </c>
+      <c r="I10" s="1">
         <v>600.0</v>
       </c>
-      <c r="I10" s="1">
-        <v>6000.0</v>
-      </c>
       <c r="J10" s="1">
-        <v>6000.0</v>
+        <v>-6000.0</v>
       </c>
       <c r="K10" s="1">
-        <v>0</v>
+        <v>6600.0</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
@@ -700,81 +706,49 @@
     </row>
     <row r="11" spans="1:15">
       <c r="B11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>10301</v>
+        <v>10206</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H11" s="1">
         <v>9000.0</v>
       </c>
       <c r="I11" s="1">
-        <v>900.0</v>
+        <v>5000.0</v>
       </c>
       <c r="J11" s="1">
-        <v>9900.0</v>
+        <v>4000.0</v>
       </c>
       <c r="K11" s="1">
-        <v>-9000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="L11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12">
-        <v>10204</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="1">
-        <v>10406.0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>-10406.0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>5000.0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>-15406.0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="H13" s="4">
-        <v>21006.0</v>
+      <c r="H12" s="7">
+        <v>13400.0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="D5:E5"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>